<commit_message>
Se aplican validaciones al inicio de sesion y se hacen comparaciones para ver si coinciden los datos ingresados del usuario con los registros actuales
</commit_message>
<xml_diff>
--- a/build/classes/datos/registros.xlsx
+++ b/build/classes/datos/registros.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>No tiene</t>
+  </si>
+  <si>
+    <t>Sebastián</t>
+  </si>
+  <si>
+    <t>Palacio</t>
+  </si>
+  <si>
+    <t>sebasx200</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>sebastian_palacio23231@elpoli,edu,co</t>
   </si>
 </sst>
 </file>
@@ -483,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE4A813-3D5E-4C16-9A49-0750FE2BAD7F}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J1"/>
@@ -585,6 +600,29 @@
         <v>19</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.00076262E9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2" xr:uid="{E6FE9982-EF6E-45D5-927F-ECC7EE23A0BA}"/>

</xml_diff>

<commit_message>
Se hace la primera version de la ventana donde los estudiantes podrán ver los docentes en una tabla
</commit_message>
<xml_diff>
--- a/build/classes/datos/registros.xlsx
+++ b/build/classes/datos/registros.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos Java\PPI_ConexionU\src\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{028FCEA5-3148-4B8D-84BF-E1812B687CC3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34096899-5BF5-4430-A95E-9B6628DFD9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15720" windowWidth="29040" xWindow="-120" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" r:id="rId1" sheetId="1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nombre</t>
   </si>
@@ -66,33 +66,6 @@
     <t>Universidad</t>
   </si>
   <si>
-    <t>Maryem</t>
-  </si>
-  <si>
-    <t>Ruiz</t>
-  </si>
-  <si>
-    <t>mruiz@elpoli.edu.co</t>
-  </si>
-  <si>
-    <t>Antioquia</t>
-  </si>
-  <si>
-    <t>Medellin</t>
-  </si>
-  <si>
-    <t>PCJIC</t>
-  </si>
-  <si>
-    <t>maryem01</t>
-  </si>
-  <si>
-    <t>P19-143</t>
-  </si>
-  <si>
-    <t>ss</t>
-  </si>
-  <si>
     <t>No tiene</t>
   </si>
   <si>
@@ -108,14 +81,13 @@
     <t>1234</t>
   </si>
   <si>
-    <t>sebastian_palacio23231@elpoli,edu,co</t>
+    <t>sebastian_palacio23231@elpoli.edu.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,26 +123,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -182,34 +147,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="registro_docente" headerRowDxfId="0" id="1" mc:Ignorable="xr xr3" name="registro_docente" ref="A1:J2" totalsRowShown="0" xr:uid="{DCFB288A-AAC6-4E6E-B46F-AAFCF4EBBD26}">
-  <autoFilter ref="A1:J2" xr:uid="{DCFB288A-AAC6-4E6E-B46F-AAFCF4EBBD26}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="Nombre" xr3:uid="{DE72D573-CD57-45C0-AE64-0975C0BD7022}"/>
-    <tableColumn id="2" name="Apellido" xr3:uid="{25D491FE-230B-4B36-B429-DA6D806250DF}"/>
-    <tableColumn id="3" name="Documento" xr3:uid="{287AFAFF-CEBC-40FB-B1A4-2AE52E407619}"/>
-    <tableColumn id="4" name="Usuario" xr3:uid="{41646C96-7294-4B85-810B-D4B4052508BC}"/>
-    <tableColumn id="5" name="Contraseña" xr3:uid="{C851BBBA-45AE-4463-9EF9-E0C482D20D8C}"/>
-    <tableColumn dataCellStyle="Hipervínculo" id="6" name="Correo" xr3:uid="{2F7D099B-912F-4979-B230-0F2154FB0FD2}"/>
-    <tableColumn id="7" name="Oficina" xr3:uid="{36A9785B-B42B-47A2-8A9C-7AD9B9BD0666}"/>
-    <tableColumn id="8" name="Departamento" xr3:uid="{18C4F0F1-FC70-45B2-BED9-2BC866684BDE}"/>
-    <tableColumn id="9" name="Ciudad" xr3:uid="{E2767882-6E16-4D4E-A90E-A6168C696C1E}"/>
-    <tableColumn id="10" name="Universidad" xr3:uid="{3F2E6D42-CE00-4403-9B43-9449897CA20E}"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -244,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -296,7 +242,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -407,21 +353,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -438,7 +384,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -490,146 +436,86 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE4A813-3D5E-4C16-9A49-0750FE2BAD7F}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE4A813-3D5E-4C16-9A49-0750FE2BAD7F}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>1000762620</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>123456789</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2">
-        <v>12345</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.00076262E9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2" xr:uid="{E6FE9982-EF6E-45D5-927F-ECC7EE23A0BA}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{ED1DE33F-ED37-4AD2-8C47-E27092637600}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se estan haciendo las validaciones del registro
</commit_message>
<xml_diff>
--- a/build/classes/datos/registros.xlsx
+++ b/build/classes/datos/registros.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos Java\PPI_ConexionU\src\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Henao\Documents\NetBeansProjects\PPI_Conexion_Poli\src\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34096899-5BF5-4430-A95E-9B6628DFD9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E2D13DA6-5F85-4899-95EE-67DE6083C86E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -82,12 +82,28 @@
   </si>
   <si>
     <t>sebastian_palacio23231@elpoli.edu.co</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>xb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,19 +139,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -152,10 +168,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -190,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -242,7 +258,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -353,21 +369,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -384,7 +400,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -436,28 +452,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE4A813-3D5E-4C16-9A49-0750FE2BAD7F}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE4A813-3D5E-4C16-9A49-0750FE2BAD7F}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -509,13 +527,59 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{ED1DE33F-ED37-4AD2-8C47-E27092637600}"/>
+    <hyperlink r:id="rId1" ref="F2" xr:uid="{ED1DE33F-ED37-4AD2-8C47-E27092637600}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se establece la navegaciòn entre las ventanas login, principal y registro
</commit_message>
<xml_diff>
--- a/build/classes/datos/registros.xlsx
+++ b/build/classes/datos/registros.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>xb</t>
+  </si>
+  <si>
+    <t>jhasbdjh</t>
+  </si>
+  <si>
+    <t>asbdjhsa</t>
+  </si>
+  <si>
+    <t>shadbjsa223</t>
+  </si>
+  <si>
+    <t>asbdsad@elpdjcn.dsbh.com</t>
   </si>
 </sst>
 </file>
@@ -460,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE4A813-3D5E-4C16-9A49-0750FE2BAD7F}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -576,6 +588,29 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2.68361723E8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2" xr:uid="{ED1DE33F-ED37-4AD2-8C47-E27092637600}"/>

</xml_diff>